<commit_message>
Initial check-in of RTx Controller Design.docx. Need explanation of ADC resolution requirements.
</commit_message>
<xml_diff>
--- a/Documentation/Component Selection/Axis Feedback LPFs.xlsx
+++ b/Documentation/Component Selection/Axis Feedback LPFs.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="61">
   <si>
     <t>Axis Position Feedback LPF’s</t>
   </si>
@@ -129,13 +129,76 @@
     <t>OPAMP2-B</t>
   </si>
   <si>
-    <t>3rd-order Sallen-Key Low-Pass Filters</t>
-  </si>
-  <si>
-    <t>Parameters:</t>
-  </si>
-  <si>
-    <t>fc</t>
+    <t>Axis Position Feedback ADC's</t>
+  </si>
+  <si>
+    <t>Ref Voltage Regulator</t>
+  </si>
+  <si>
+    <t>C1</t>
+  </si>
+  <si>
+    <t>C4</t>
+  </si>
+  <si>
+    <t>C5</t>
+  </si>
+  <si>
+    <t>ADC1</t>
+  </si>
+  <si>
+    <t>C2</t>
+  </si>
+  <si>
+    <t>C6</t>
+  </si>
+  <si>
+    <t>C7</t>
+  </si>
+  <si>
+    <t>ADC2</t>
+  </si>
+  <si>
+    <t>C3</t>
+  </si>
+  <si>
+    <t>C8</t>
+  </si>
+  <si>
+    <t>C9</t>
+  </si>
+  <si>
+    <t>R16</t>
+  </si>
+  <si>
+    <t>ADC3</t>
+  </si>
+  <si>
+    <t>C40</t>
+  </si>
+  <si>
+    <t>C41</t>
+  </si>
+  <si>
+    <t>C42</t>
+  </si>
+  <si>
+    <t>R20</t>
+  </si>
+  <si>
+    <t>ADC4</t>
+  </si>
+  <si>
+    <t>C23</t>
+  </si>
+  <si>
+    <t>C24</t>
+  </si>
+  <si>
+    <t>C25</t>
+  </si>
+  <si>
+    <t>REF1</t>
   </si>
 </sst>
 </file>
@@ -159,7 +222,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -167,14 +230,33 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -470,218 +552,269 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="B2:E38"/>
+  <dimension ref="B2:T12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+    <sheetView tabSelected="1" topLeftCell="L1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="M12" sqref="M12:P12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="2" max="2" width="5.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="5.7109375" style="3" bestFit="1" customWidth="1"/>
+    <col min="3" max="9" width="4.140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="5.7109375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="20.5703125" style="3" bestFit="1" customWidth="1"/>
+    <col min="13" max="15" width="4.140625" bestFit="1" customWidth="1"/>
+    <col min="16" max="17" width="5.7109375" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="4.140625" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="5.7109375" bestFit="1" customWidth="1"/>
+    <col min="21" max="23" width="3.140625" bestFit="1" customWidth="1"/>
+    <col min="24" max="27" width="4.140625" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="5.7109375" bestFit="1" customWidth="1"/>
+    <col min="30" max="36" width="4.140625" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="10.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:5">
-      <c r="B2" s="1" t="s">
+    <row r="2" spans="2:20">
+      <c r="B2" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="1"/>
-      <c r="D2" s="1"/>
-      <c r="E2" s="1"/>
-    </row>
-    <row r="3" spans="2:5">
-      <c r="B3" t="s">
+      <c r="C2" s="2"/>
+      <c r="D2" s="2"/>
+      <c r="E2" s="2"/>
+      <c r="F2" s="2"/>
+      <c r="G2" s="2"/>
+      <c r="H2" s="2"/>
+      <c r="I2" s="2"/>
+      <c r="J2" s="2"/>
+      <c r="L2" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="M2" s="2"/>
+      <c r="N2" s="2"/>
+      <c r="O2" s="2"/>
+      <c r="P2" s="2"/>
+      <c r="Q2" s="2"/>
+      <c r="R2" s="2"/>
+      <c r="S2" s="2"/>
+      <c r="T2" s="2"/>
+    </row>
+    <row r="3" spans="2:20">
+      <c r="B3" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="E3" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="4" spans="2:5">
-      <c r="C4" t="s">
+      <c r="L3" s="3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="2:20">
+      <c r="C4" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="E4" t="s">
+      <c r="D4" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I4" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J4" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="M4" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="N4" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="O4" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="P4" s="1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="5" spans="2:20">
+      <c r="B5" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="L5" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" spans="2:20">
+      <c r="C6" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="H6" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="I6" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="J6" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="M6" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="N6" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="O6" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="P6" s="1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="7" spans="2:20">
+      <c r="B7" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="L7" s="3" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="8" spans="2:20">
+      <c r="C8" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="G8" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="H8" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="I8" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="J8" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="M8" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="N8" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="O8" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="P8" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="Q8" s="1" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="9" spans="2:20">
+      <c r="B9" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="L9" s="3" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="10" spans="2:20">
+      <c r="C10" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="G10" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="H10" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="I10" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="J10" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="M10" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="N10" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="O10" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="P10" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="Q10" s="1" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="11" spans="2:20">
+      <c r="L11" s="3" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="5" spans="2:5">
-      <c r="C5" t="s">
-        <v>3</v>
-      </c>
-      <c r="E5" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="6" spans="2:5">
-      <c r="C6" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="7" spans="2:5">
-      <c r="C7" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="8" spans="2:5">
-      <c r="C8" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="9" spans="2:5">
-      <c r="C9" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="10" spans="2:5">
-      <c r="C10" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="11" spans="2:5">
-      <c r="C11" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="12" spans="2:5">
-      <c r="B12" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="13" spans="2:5">
-      <c r="C13" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="14" spans="2:5">
-      <c r="C14" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="15" spans="2:5">
-      <c r="C15" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="16" spans="2:5">
-      <c r="C16" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="17" spans="2:3">
-      <c r="C17" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="18" spans="2:3">
-      <c r="C18" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="19" spans="2:3">
-      <c r="C19" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="20" spans="2:3">
-      <c r="C20" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="21" spans="2:3">
-      <c r="B21" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="22" spans="2:3">
-      <c r="C22" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="23" spans="2:3">
-      <c r="C23" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="24" spans="2:3">
-      <c r="C24" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="25" spans="2:3">
-      <c r="C25" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="26" spans="2:3">
-      <c r="C26" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="27" spans="2:3">
-      <c r="C27" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="28" spans="2:3">
-      <c r="C28" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="29" spans="2:3">
-      <c r="C29" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="30" spans="2:3">
-      <c r="B30" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="31" spans="2:3">
-      <c r="C31" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="32" spans="2:3">
-      <c r="C32" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="33" spans="3:3">
-      <c r="C33" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="34" spans="3:3">
-      <c r="C34" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="35" spans="3:3">
-      <c r="C35" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="36" spans="3:3">
-      <c r="C36" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="37" spans="3:3">
-      <c r="C37" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="38" spans="3:3">
-      <c r="C38" t="s">
-        <v>36</v>
+    <row r="12" spans="2:20">
+      <c r="M12" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="N12" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="O12" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="P12" s="1" t="s">
+        <v>60</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="B2:E2"/>
+  <mergeCells count="2">
+    <mergeCell ref="B2:J2"/>
+    <mergeCell ref="L2:T2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>